<commit_message>
fix retrieval sample.xlsx format issue
Signed-off-by: Lv, Liang1 <liang1.lv@intel.com>
</commit_message>
<xml_diff>
--- a/intel_extension_for_transformers/neural_chat/assets/docs/sample.xlsx
+++ b/intel_extension_for_transformers/neural_chat/assets/docs/sample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://intel-my.sharepoint.com/personal/xuhui_ren_intel_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xuhuiren\OneDrive - Intel Corporation\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_F25DC773A252ABDACC104862895C4EF45ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D807E3CD-FE2E-47BF-811B-FBE11AE6E40C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF251A06-3E21-461B-9C85-78781551F769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32100" yWindow="6000" windowWidth="28800" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,16 +27,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Question</t>
-  </si>
-  <si>
-    <t>Answer</t>
-  </si>
-  <si>
     <t>Who is the CEO of Intel?</t>
   </si>
   <si>
     <t>Patrick P. Gelsinger</t>
+  </si>
+  <si>
+    <t>Questions</t>
+  </si>
+  <si>
+    <t>Answers</t>
   </si>
 </sst>
 </file>
@@ -360,7 +360,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -371,18 +371,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enable NeuralChat Unit Test process (#195)
</commit_message>
<xml_diff>
--- a/intel_extension_for_transformers/neural_chat/assets/docs/sample.xlsx
+++ b/intel_extension_for_transformers/neural_chat/assets/docs/sample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://intel-my.sharepoint.com/personal/xuhui_ren_intel_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xuhuiren\OneDrive - Intel Corporation\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_F25DC773A252ABDACC104862895C4EF45ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D807E3CD-FE2E-47BF-811B-FBE11AE6E40C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF251A06-3E21-461B-9C85-78781551F769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32100" yWindow="6000" windowWidth="28800" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,16 +27,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Question</t>
-  </si>
-  <si>
-    <t>Answer</t>
-  </si>
-  <si>
     <t>Who is the CEO of Intel?</t>
   </si>
   <si>
     <t>Patrick P. Gelsinger</t>
+  </si>
+  <si>
+    <t>Questions</t>
+  </si>
+  <si>
+    <t>Answers</t>
   </si>
 </sst>
 </file>
@@ -360,7 +360,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -371,18 +371,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>